<commit_message>
fixed joint angle names
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="163" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="202" uniqueCount="48">
   <si>
     <t>JointMotion</t>
   </si>
@@ -139,6 +139,24 @@
   </si>
   <si>
     <t>rest</t>
+  </si>
+  <si>
+    <t>L5S1LateralBending</t>
+  </si>
+  <si>
+    <t>L5S1AxialBending</t>
+  </si>
+  <si>
+    <t>L5S1Flexion_Extension</t>
+  </si>
+  <si>
+    <t>T1C7LateralBending</t>
+  </si>
+  <si>
+    <t>T1C7AxialRotation</t>
+  </si>
+  <si>
+    <t>T1C7Flexion_Extension</t>
   </si>
 </sst>
 </file>
@@ -192,7 +210,7 @@
   <cols>
     <col min="1" max="1" width="39.42578125" customWidth="true"/>
     <col min="2" max="2" width="14.42578125" customWidth="true"/>
-    <col min="3" max="3" width="12.42578125" customWidth="true"/>
+    <col min="3" max="3" width="14.42578125" customWidth="true"/>
     <col min="4" max="4" width="11.7109375" customWidth="true"/>
     <col min="5" max="5" width="20.85546875" customWidth="true"/>
     <col min="6" max="6" width="20.85546875" customWidth="true"/>
@@ -232,698 +250,698 @@
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>1</v>
+        <v>42</v>
       </c>
       <c r="B2" s="0">
-        <v>1.2881402780399251</v>
+        <v>0.056855999578991998</v>
       </c>
       <c r="C2" s="0">
-        <v>-13.085612019136001</v>
+        <v>-5.6480445169226803</v>
       </c>
       <c r="D2" s="0">
-        <v>16.284036456297599</v>
+        <v>7.0412429546582498</v>
       </c>
       <c r="E2" s="0">
         <v>0</v>
       </c>
       <c r="F2" s="0">
-        <v>62.421524663677133</v>
+        <v>51.603139013452918</v>
       </c>
       <c r="G2" s="0">
-        <v>1.5246636771300448</v>
+        <v>0</v>
       </c>
       <c r="H2" s="0">
-        <v>48.890134529147986</v>
+        <v>51.00896860986547</v>
       </c>
       <c r="I2" s="0">
-        <v>63.946188340807176</v>
+        <v>51.603139013452918</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>2</v>
+        <v>43</v>
       </c>
       <c r="B3" s="0">
-        <v>-3.2570850851399102</v>
+        <v>-0.633438368987296</v>
       </c>
       <c r="C3" s="0">
-        <v>-31.791243506666</v>
+        <v>-6.7370539325142396</v>
       </c>
       <c r="D3" s="0">
-        <v>36.544345532974603</v>
+        <v>10.534483820659901</v>
       </c>
       <c r="E3" s="0">
         <v>0</v>
       </c>
       <c r="F3" s="0">
-        <v>22.387892376681613</v>
+        <v>32.376681614349778</v>
       </c>
       <c r="G3" s="0">
-        <v>10.336322869955158</v>
+        <v>0.14573991031390135</v>
       </c>
       <c r="H3" s="0">
-        <v>14.428251121076233</v>
+        <v>31.434977578475337</v>
       </c>
       <c r="I3" s="0">
-        <v>32.724215246636774</v>
+        <v>32.522421524663677</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>3</v>
+        <v>44</v>
       </c>
       <c r="B4" s="0">
-        <v>-16.892853595201998</v>
+        <v>5.0405226390416402</v>
       </c>
       <c r="C4" s="0">
-        <v>-36.257618053616397</v>
+        <v>-3.1545423845062102</v>
       </c>
       <c r="D4" s="0">
-        <v>3.2265079893410702</v>
+        <v>15.5669831340496</v>
       </c>
       <c r="E4" s="0">
         <v>0</v>
       </c>
       <c r="F4" s="0">
-        <v>5.5269058295964122</v>
+        <v>93.374439461883412</v>
       </c>
       <c r="G4" s="0">
-        <v>0</v>
+        <v>3.8677130044843051</v>
       </c>
       <c r="H4" s="0">
-        <v>5.5269058295964122</v>
+        <v>46.188340807174889</v>
       </c>
       <c r="I4" s="0">
-        <v>5.5269058295964122</v>
+        <v>97.242152466367713</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="0" t="s">
-        <v>4</v>
+        <v>45</v>
       </c>
       <c r="B5" s="0">
-        <v>2.6367995491075948</v>
+        <v>0.90970031547938601</v>
       </c>
       <c r="C5" s="0">
-        <v>-16.641324222296898</v>
+        <v>-10.0804170126939</v>
       </c>
       <c r="D5" s="0">
-        <v>39.624096991770401</v>
+        <v>11.0576417761608</v>
       </c>
       <c r="E5" s="0">
         <v>0</v>
       </c>
       <c r="F5" s="0">
-        <v>32.107623318385656</v>
+        <v>32.41031390134529</v>
       </c>
       <c r="G5" s="0">
-        <v>58.553811659192824</v>
+        <v>67.58968609865471</v>
       </c>
       <c r="H5" s="0">
-        <v>0.3026905829596413</v>
+        <v>0</v>
       </c>
       <c r="I5" s="0">
-        <v>90.66143497757848</v>
+        <v>100</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="0" t="s">
-        <v>5</v>
+        <v>46</v>
       </c>
       <c r="B6" s="0">
-        <v>12.8098924780892</v>
+        <v>-1.5269556313914749</v>
       </c>
       <c r="C6" s="0">
-        <v>-29.6647045906656</v>
+        <v>-15.4261599447617</v>
       </c>
       <c r="D6" s="0">
-        <v>71.155218608347397</v>
+        <v>18.286292167347298</v>
       </c>
       <c r="E6" s="0">
         <v>0</v>
       </c>
       <c r="F6" s="0">
-        <v>17.230941704035875</v>
+        <v>62.511210762331835</v>
       </c>
       <c r="G6" s="0">
-        <v>35.156950672645742</v>
+        <v>36.423766816143498</v>
       </c>
       <c r="H6" s="0">
-        <v>3.2062780269058297</v>
+        <v>0.49327354260089684</v>
       </c>
       <c r="I6" s="0">
-        <v>52.38789237668162</v>
+        <v>98.934977578475326</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="0" t="s">
-        <v>6</v>
+        <v>47</v>
       </c>
       <c r="B7" s="0">
-        <v>23.279145750004453</v>
+        <v>10.2969425162633</v>
       </c>
       <c r="C7" s="0">
-        <v>-33.265334355849099</v>
+        <v>-0.071126321208431903</v>
       </c>
       <c r="D7" s="0">
-        <v>90.5826288220713</v>
+        <v>21.116451303800201</v>
       </c>
       <c r="E7" s="0">
         <v>0</v>
       </c>
       <c r="F7" s="0">
-        <v>0.3811659192825112</v>
+        <v>0.056053811659192827</v>
       </c>
       <c r="G7" s="0">
-        <v>22.118834080717491</v>
+        <v>86.311659192825104</v>
       </c>
       <c r="H7" s="0">
-        <v>0.50448430493273544</v>
+        <v>0</v>
       </c>
       <c r="I7" s="0">
-        <v>22.500000000000004</v>
+        <v>86.367713004484301</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="0" t="s">
-        <v>7</v>
+        <v>4</v>
       </c>
       <c r="B8" s="0">
-        <v>-4.56697248682321</v>
+        <v>2.6367995491075948</v>
       </c>
       <c r="C8" s="0">
-        <v>-82.884122257430306</v>
+        <v>-16.641324222296898</v>
       </c>
       <c r="D8" s="0">
-        <v>45.405435656246297</v>
+        <v>39.624096991770401</v>
       </c>
       <c r="E8" s="0">
         <v>0</v>
       </c>
       <c r="F8" s="0">
-        <v>19.618834080717491</v>
+        <v>32.107623318385656</v>
       </c>
       <c r="G8" s="0">
-        <v>23.934977578475337</v>
+        <v>58.553811659192824</v>
       </c>
       <c r="H8" s="0">
-        <v>23.183856502242154</v>
+        <v>0.3026905829596413</v>
       </c>
       <c r="I8" s="0">
-        <v>43.553811659192831</v>
+        <v>90.66143497757848</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="0" t="s">
-        <v>8</v>
+        <v>5</v>
       </c>
       <c r="B9" s="0">
-        <v>67.035729272602353</v>
+        <v>12.8098924780892</v>
       </c>
       <c r="C9" s="0">
-        <v>-65.772343902386694</v>
+        <v>-29.6647045906656</v>
       </c>
       <c r="D9" s="0">
-        <v>174.73185673422799</v>
+        <v>71.155218608347397</v>
       </c>
       <c r="E9" s="0">
         <v>0</v>
       </c>
       <c r="F9" s="0">
-        <v>2.5560538116591927</v>
+        <v>17.230941704035875</v>
       </c>
       <c r="G9" s="0">
-        <v>5.0560538116591927</v>
+        <v>35.156950672645742</v>
       </c>
       <c r="H9" s="0">
-        <v>0.99775784753363228</v>
+        <v>3.2062780269058297</v>
       </c>
       <c r="I9" s="0">
-        <v>7.6121076233183853</v>
+        <v>52.38789237668162</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="0" t="s">
-        <v>9</v>
+        <v>6</v>
       </c>
       <c r="B10" s="0">
-        <v>44.222785814108704</v>
+        <v>23.279145750004453</v>
       </c>
       <c r="C10" s="0">
-        <v>-52.468041020853804</v>
+        <v>-33.265334355849099</v>
       </c>
       <c r="D10" s="0">
-        <v>159.98850067244601</v>
+        <v>90.5826288220713</v>
       </c>
       <c r="E10" s="0">
         <v>0</v>
       </c>
       <c r="F10" s="0">
-        <v>3.3632286995515694</v>
+        <v>0.3811659192825112</v>
       </c>
       <c r="G10" s="0">
-        <v>29.192825112107624</v>
+        <v>22.118834080717491</v>
       </c>
       <c r="H10" s="0">
-        <v>0.3026905829596413</v>
+        <v>0.50448430493273544</v>
       </c>
       <c r="I10" s="0">
-        <v>32.55605381165919</v>
+        <v>22.500000000000004</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="0" t="s">
-        <v>10</v>
+        <v>7</v>
       </c>
       <c r="B11" s="0">
-        <v>5.5241928379928957</v>
+        <v>-4.56697248682321</v>
       </c>
       <c r="C11" s="0">
-        <v>-89.425096386377106</v>
+        <v>-82.884122257430306</v>
       </c>
       <c r="D11" s="0">
-        <v>87.583824191846503</v>
+        <v>45.405435656246297</v>
       </c>
       <c r="E11" s="0">
-        <v>0</v>
+        <v>23.183856502242154</v>
       </c>
       <c r="F11" s="0">
-        <v>15.078475336322869</v>
+        <v>19.618834080717491</v>
       </c>
       <c r="G11" s="0">
-        <v>15.011210762331839</v>
+        <v>23.934977578475337</v>
       </c>
       <c r="H11" s="0">
-        <v>13.778026905829597</v>
+        <v>0</v>
       </c>
       <c r="I11" s="0">
-        <v>30.08968609865471</v>
+        <v>66.737668161434982</v>
       </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
-        <v>11</v>
+        <v>8</v>
       </c>
       <c r="B12" s="0">
-        <v>42.217495777057451</v>
+        <v>67.035729272602353</v>
       </c>
       <c r="C12" s="0">
-        <v>-179.599138863013</v>
+        <v>-65.772343902386694</v>
       </c>
       <c r="D12" s="0">
-        <v>179.490232518791</v>
+        <v>174.73185673422799</v>
       </c>
       <c r="E12" s="0">
-        <v>0</v>
+        <v>0.99775784753363228</v>
       </c>
       <c r="F12" s="0">
-        <v>7.6681614349775788</v>
+        <v>2.5560538116591927</v>
       </c>
       <c r="G12" s="0">
-        <v>8.9125560538116577</v>
+        <v>5.0560538116591927</v>
       </c>
       <c r="H12" s="0">
-        <v>9.4843049327354247</v>
+        <v>0</v>
       </c>
       <c r="I12" s="0">
-        <v>16.580717488789237</v>
+        <v>8.6098654708520179</v>
       </c>
     </row>
     <row r="13">
       <c r="A13" s="0" t="s">
-        <v>12</v>
+        <v>9</v>
       </c>
       <c r="B13" s="0">
-        <v>-21.810325391650149</v>
+        <v>44.222785814108704</v>
       </c>
       <c r="C13" s="0">
-        <v>-179.99997391993301</v>
+        <v>-52.468041020853804</v>
       </c>
       <c r="D13" s="0">
-        <v>179.77469146537999</v>
+        <v>159.98850067244601</v>
       </c>
       <c r="E13" s="0">
-        <v>0</v>
+        <v>0.3026905829596413</v>
       </c>
       <c r="F13" s="0">
-        <v>13.307174887892376</v>
+        <v>3.3632286995515694</v>
       </c>
       <c r="G13" s="0">
-        <v>6.9730941704035878</v>
+        <v>29.192825112107624</v>
       </c>
       <c r="H13" s="0">
-        <v>14.013452914798204</v>
+        <v>0</v>
       </c>
       <c r="I13" s="0">
-        <v>20.280269058295964</v>
+        <v>32.858744394618832</v>
       </c>
     </row>
     <row r="14">
       <c r="A14" s="0" t="s">
-        <v>13</v>
+        <v>10</v>
       </c>
       <c r="B14" s="0">
-        <v>7.740036771974105</v>
+        <v>5.5241928379928957</v>
       </c>
       <c r="C14" s="0">
-        <v>-21.820556950950401</v>
+        <v>-89.425096386377106</v>
       </c>
       <c r="D14" s="0">
-        <v>47.036644219330299</v>
+        <v>87.583824191846503</v>
       </c>
       <c r="E14" s="0">
-        <v>1.3228699551569507</v>
+        <v>13.778026905829597</v>
       </c>
       <c r="F14" s="0">
-        <v>31.468609865470853</v>
+        <v>15.078475336322869</v>
       </c>
       <c r="G14" s="0">
-        <v>58.789237668161434</v>
+        <v>15.011210762331839</v>
       </c>
       <c r="H14" s="0">
         <v>0</v>
       </c>
       <c r="I14" s="0">
-        <v>91.580717488789247</v>
+        <v>43.867713004484301</v>
       </c>
     </row>
     <row r="15">
       <c r="A15" s="0" t="s">
-        <v>14</v>
+        <v>11</v>
       </c>
       <c r="B15" s="0">
-        <v>13.7713796105868</v>
+        <v>42.217495777057451</v>
       </c>
       <c r="C15" s="0">
-        <v>-43.728449213337299</v>
+        <v>-179.599138863013</v>
       </c>
       <c r="D15" s="0">
-        <v>56.908493492938</v>
+        <v>179.490232518791</v>
       </c>
       <c r="E15" s="0">
-        <v>4.2600896860986541</v>
+        <v>9.4843049327354247</v>
       </c>
       <c r="F15" s="0">
-        <v>23.811659192825115</v>
+        <v>7.6681614349775788</v>
       </c>
       <c r="G15" s="0">
-        <v>31.704035874439462</v>
+        <v>8.9125560538116577</v>
       </c>
       <c r="H15" s="0">
         <v>0</v>
       </c>
       <c r="I15" s="0">
-        <v>59.775784753363233</v>
+        <v>26.06502242152466</v>
       </c>
     </row>
     <row r="16">
       <c r="A16" s="0" t="s">
-        <v>15</v>
+        <v>12</v>
       </c>
       <c r="B16" s="0">
-        <v>21.9341946313397</v>
+        <v>-21.810325391650149</v>
       </c>
       <c r="C16" s="0">
-        <v>-44.891381586050301</v>
+        <v>-179.99997391993301</v>
       </c>
       <c r="D16" s="0">
-        <v>83.838028371070294</v>
+        <v>179.77469146537999</v>
       </c>
       <c r="E16" s="0">
-        <v>0.72869955156950672</v>
+        <v>14.013452914798204</v>
       </c>
       <c r="F16" s="0">
-        <v>5.4372197309417034</v>
+        <v>13.307174887892376</v>
       </c>
       <c r="G16" s="0">
-        <v>36.143497757847534</v>
+        <v>6.9730941704035878</v>
       </c>
       <c r="H16" s="0">
         <v>0</v>
       </c>
       <c r="I16" s="0">
-        <v>42.309417040358746</v>
+        <v>34.293721973094165</v>
       </c>
     </row>
     <row r="17">
       <c r="A17" s="0" t="s">
-        <v>16</v>
+        <v>13</v>
       </c>
       <c r="B17" s="0">
-        <v>-9.5844571068494062</v>
+        <v>7.740036771974105</v>
       </c>
       <c r="C17" s="0">
-        <v>-75.485737677646497</v>
+        <v>-21.820556950950401</v>
       </c>
       <c r="D17" s="0">
-        <v>35.539988122927497</v>
+        <v>47.036644219330299</v>
       </c>
       <c r="E17" s="0">
-        <v>24.854260089686097</v>
+        <v>0</v>
       </c>
       <c r="F17" s="0">
-        <v>21.154708520179373</v>
+        <v>31.468609865470853</v>
       </c>
       <c r="G17" s="0">
-        <v>31.401345291479821</v>
+        <v>58.789237668161434</v>
       </c>
       <c r="H17" s="0">
-        <v>0</v>
+        <v>1.3228699551569507</v>
       </c>
       <c r="I17" s="0">
-        <v>77.41031390134529</v>
+        <v>90.257847533632287</v>
       </c>
     </row>
     <row r="18">
       <c r="A18" s="0" t="s">
-        <v>17</v>
+        <v>14</v>
       </c>
       <c r="B18" s="0">
-        <v>66.030571124831695</v>
+        <v>13.7713796105868</v>
       </c>
       <c r="C18" s="0">
-        <v>-31.923995841788599</v>
+        <v>-43.728449213337299</v>
       </c>
       <c r="D18" s="0">
-        <v>137.96940114528701</v>
+        <v>56.908493492938</v>
       </c>
       <c r="E18" s="0">
-        <v>3.340807174887892</v>
+        <v>0</v>
       </c>
       <c r="F18" s="0">
-        <v>9.8094170403587455</v>
+        <v>23.811659192825115</v>
       </c>
       <c r="G18" s="0">
-        <v>6.9058295964125564</v>
+        <v>31.704035874439462</v>
       </c>
       <c r="H18" s="0">
-        <v>0</v>
+        <v>4.2600896860986541</v>
       </c>
       <c r="I18" s="0">
-        <v>20.056053811659194</v>
+        <v>55.515695067264573</v>
       </c>
     </row>
     <row r="19">
       <c r="A19" s="0" t="s">
-        <v>18</v>
+        <v>15</v>
       </c>
       <c r="B19" s="0">
-        <v>47.877689839817904</v>
+        <v>21.9341946313397</v>
       </c>
       <c r="C19" s="0">
-        <v>-13.3801218979171</v>
+        <v>-44.891381586050301</v>
       </c>
       <c r="D19" s="0">
-        <v>152.42691614070401</v>
+        <v>83.838028371070294</v>
       </c>
       <c r="E19" s="0">
-        <v>0</v>
+        <v>0.72869955156950672</v>
       </c>
       <c r="F19" s="0">
-        <v>8.2286995515695072</v>
+        <v>5.4372197309417034</v>
       </c>
       <c r="G19" s="0">
-        <v>24.585201793721971</v>
+        <v>36.143497757847534</v>
       </c>
       <c r="H19" s="0">
         <v>0</v>
       </c>
       <c r="I19" s="0">
-        <v>32.813901345291477</v>
+        <v>42.309417040358746</v>
       </c>
     </row>
     <row r="20">
       <c r="A20" s="0" t="s">
-        <v>19</v>
+        <v>16</v>
       </c>
       <c r="B20" s="0">
-        <v>3.1766172690525947</v>
+        <v>-9.5844571068494062</v>
       </c>
       <c r="C20" s="0">
-        <v>-83.945123560199306</v>
+        <v>-75.485737677646497</v>
       </c>
       <c r="D20" s="0">
-        <v>87.341748097180002</v>
+        <v>35.539988122927497</v>
       </c>
       <c r="E20" s="0">
-        <v>0</v>
+        <v>24.854260089686097</v>
       </c>
       <c r="F20" s="0">
-        <v>15.538116591928249</v>
+        <v>21.154708520179373</v>
       </c>
       <c r="G20" s="0">
-        <v>11.165919282511211</v>
+        <v>31.401345291479821</v>
       </c>
       <c r="H20" s="0">
-        <v>17.993273542600896</v>
+        <v>0</v>
       </c>
       <c r="I20" s="0">
-        <v>26.704035874439462</v>
+        <v>77.41031390134529</v>
       </c>
     </row>
     <row r="21">
       <c r="A21" s="0" t="s">
-        <v>20</v>
+        <v>17</v>
       </c>
       <c r="B21" s="0">
-        <v>54.950154444605346</v>
+        <v>66.030571124831695</v>
       </c>
       <c r="C21" s="0">
-        <v>-179.99462121883499</v>
+        <v>-31.923995841788599</v>
       </c>
       <c r="D21" s="0">
-        <v>179.965373349917</v>
+        <v>137.96940114528701</v>
       </c>
       <c r="E21" s="0">
-        <v>0</v>
+        <v>3.340807174887892</v>
       </c>
       <c r="F21" s="0">
-        <v>7.4551569506726452</v>
+        <v>9.8094170403587455</v>
       </c>
       <c r="G21" s="0">
-        <v>8.4304932735426004</v>
+        <v>6.9058295964125564</v>
       </c>
       <c r="H21" s="0">
-        <v>7.2197309417040358</v>
+        <v>0</v>
       </c>
       <c r="I21" s="0">
-        <v>15.885650224215246</v>
+        <v>20.056053811659194</v>
       </c>
     </row>
     <row r="22">
       <c r="A22" s="0" t="s">
-        <v>21</v>
+        <v>18</v>
       </c>
       <c r="B22" s="0">
-        <v>-23.730004712883851</v>
+        <v>47.877689839817904</v>
       </c>
       <c r="C22" s="0">
-        <v>-179.936453743854</v>
+        <v>-13.3801218979171</v>
       </c>
       <c r="D22" s="0">
-        <v>179.81342543044599</v>
+        <v>152.42691614070401</v>
       </c>
       <c r="E22" s="0">
-        <v>11.098654708520179</v>
+        <v>0</v>
       </c>
       <c r="F22" s="0">
-        <v>12.275784753363228</v>
+        <v>8.2286995515695072</v>
       </c>
       <c r="G22" s="0">
-        <v>6.3340807174887894</v>
+        <v>24.585201793721971</v>
       </c>
       <c r="H22" s="0">
         <v>0</v>
       </c>
       <c r="I22" s="0">
-        <v>29.708520179372194</v>
+        <v>32.813901345291477</v>
       </c>
     </row>
     <row r="23">
       <c r="A23" s="0" t="s">
-        <v>22</v>
+        <v>19</v>
       </c>
       <c r="B23" s="0">
-        <v>2.4914987360676051</v>
+        <v>3.1766172690525947</v>
       </c>
       <c r="C23" s="0">
-        <v>-12.468462349786799</v>
+        <v>-83.945123560199306</v>
       </c>
       <c r="D23" s="0">
-        <v>22.947562512428501</v>
+        <v>87.341748097180002</v>
       </c>
       <c r="E23" s="0">
-        <v>1.2556053811659191</v>
+        <v>17.993273542600896</v>
       </c>
       <c r="F23" s="0">
-        <v>32.5</v>
+        <v>15.538116591928249</v>
       </c>
       <c r="G23" s="0">
-        <v>41.58071748878924</v>
+        <v>11.165919282511211</v>
       </c>
       <c r="H23" s="0">
         <v>0</v>
       </c>
       <c r="I23" s="0">
-        <v>75.336322869955154</v>
+        <v>44.697309417040358</v>
       </c>
     </row>
     <row r="24">
       <c r="A24" s="0" t="s">
-        <v>23</v>
+        <v>20</v>
       </c>
       <c r="B24" s="0">
-        <v>-2.93216545520451</v>
+        <v>54.950154444605346</v>
       </c>
       <c r="C24" s="0">
-        <v>-28.035435180514099</v>
+        <v>-179.99462121883499</v>
       </c>
       <c r="D24" s="0">
-        <v>15.184883681118899</v>
+        <v>179.965373349917</v>
       </c>
       <c r="E24" s="0">
-        <v>19.338565022421523</v>
+        <v>7.2197309417040358</v>
       </c>
       <c r="F24" s="0">
-        <v>45.235426008968609</v>
+        <v>7.4551569506726452</v>
       </c>
       <c r="G24" s="0">
-        <v>31.008968609865473</v>
+        <v>8.4304932735426004</v>
       </c>
       <c r="H24" s="0">
         <v>0</v>
       </c>
       <c r="I24" s="0">
-        <v>95.582959641255613</v>
+        <v>23.105381165919283</v>
       </c>
     </row>
     <row r="25">
       <c r="A25" s="0" t="s">
-        <v>24</v>
+        <v>21</v>
       </c>
       <c r="B25" s="0">
-        <v>7.6166047378313451</v>
+        <v>-23.730004712883851</v>
       </c>
       <c r="C25" s="0">
-        <v>-21.343960409019299</v>
+        <v>-179.936453743854</v>
       </c>
       <c r="D25" s="0">
-        <v>106.80244021127901</v>
+        <v>179.81342543044599</v>
       </c>
       <c r="E25" s="0">
-        <v>2.9484304932735426</v>
+        <v>11.098654708520179</v>
       </c>
       <c r="F25" s="0">
-        <v>17.847533632286996</v>
+        <v>12.275784753363228</v>
       </c>
       <c r="G25" s="0">
-        <v>38.778026905829599</v>
+        <v>6.3340807174887894</v>
       </c>
       <c r="H25" s="0">
         <v>0</v>
       </c>
       <c r="I25" s="0">
-        <v>59.573991031390136</v>
+        <v>29.708520179372194</v>
       </c>
     </row>
     <row r="26">
@@ -969,7 +987,7 @@
         <v>17.911360789958199</v>
       </c>
       <c r="E27" s="0">
-        <v>14.786995515695068</v>
+        <v>0</v>
       </c>
       <c r="F27" s="0">
         <v>71.782511210762337</v>
@@ -978,10 +996,10 @@
         <v>13.239910313901346</v>
       </c>
       <c r="H27" s="0">
-        <v>0</v>
+        <v>14.786995515695068</v>
       </c>
       <c r="I27" s="0">
-        <v>99.809417040358753</v>
+        <v>85.022421524663685</v>
       </c>
     </row>
     <row r="28">
@@ -1015,89 +1033,89 @@
     </row>
     <row r="29">
       <c r="A29" s="0" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="B29" s="0">
-        <v>2.5423229063357349</v>
+        <v>-0.08530494418099005</v>
       </c>
       <c r="C29" s="0">
-        <v>-11.696126454453299</v>
+        <v>-10.165825057581699</v>
       </c>
       <c r="D29" s="0">
-        <v>28.629645543264701</v>
+        <v>11.8575857434467</v>
       </c>
       <c r="E29" s="0">
         <v>0</v>
       </c>
       <c r="F29" s="0">
-        <v>12.208520179372197</v>
+        <v>48.206278026905828</v>
       </c>
       <c r="G29" s="0">
-        <v>52.253363228699556</v>
+        <v>0.2802690582959641</v>
       </c>
       <c r="H29" s="0">
-        <v>0</v>
+        <v>51.479820627802688</v>
       </c>
       <c r="I29" s="0">
-        <v>64.461883408071756</v>
+        <v>48.486547085201792</v>
       </c>
     </row>
     <row r="30">
       <c r="A30" s="0" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
       <c r="B30" s="0">
-        <v>-4.2649108888336853</v>
+        <v>-0.83586032287941747</v>
       </c>
       <c r="C30" s="0">
-        <v>-31.439304426620001</v>
+        <v>-17.5751832524092</v>
       </c>
       <c r="D30" s="0">
-        <v>20.035654902258401</v>
+        <v>18.901197932947198</v>
       </c>
       <c r="E30" s="0">
         <v>0</v>
       </c>
       <c r="F30" s="0">
-        <v>38.688340807174889</v>
+        <v>37.040358744394617</v>
       </c>
       <c r="G30" s="0">
-        <v>39.932735426008968</v>
+        <v>2.5</v>
       </c>
       <c r="H30" s="0">
-        <v>7.7130044843049337</v>
+        <v>58.867713004484301</v>
       </c>
       <c r="I30" s="0">
-        <v>78.621076233183857</v>
+        <v>39.540358744394617</v>
       </c>
     </row>
     <row r="31">
       <c r="A31" s="0" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B31" s="0">
-        <v>7.3809446875154352</v>
+        <v>16.580742738412852</v>
       </c>
       <c r="C31" s="0">
-        <v>-20.038799891856801</v>
+        <v>1.03325845525986</v>
       </c>
       <c r="D31" s="0">
-        <v>115.501371600556</v>
+        <v>156.51753593351799</v>
       </c>
       <c r="E31" s="0">
-        <v>0.3811659192825112</v>
+        <v>0</v>
       </c>
       <c r="F31" s="0">
-        <v>14.730941704035875</v>
+        <v>32.253363228699548</v>
       </c>
       <c r="G31" s="0">
-        <v>29.360986547085201</v>
+        <v>26.939461883408072</v>
       </c>
       <c r="H31" s="0">
         <v>0</v>
       </c>
       <c r="I31" s="0">
-        <v>44.473094170403584</v>
+        <v>59.19282511210762</v>
       </c>
     </row>
     <row r="32">

</xml_diff>

<commit_message>
test_excel and third arraying
</commit_message>
<xml_diff>
--- a/results.xlsx
+++ b/results.xlsx
@@ -13,7 +13,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="471" uniqueCount="53">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" count="510" uniqueCount="53">
   <si>
     <t>JointMotion</t>
   </si>
@@ -223,12 +223,12 @@
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15"/>
   <cols>
-    <col min="1" max="1" width="32" customWidth="true"/>
+    <col min="1" max="1" width="39.42578125" customWidth="true"/>
     <col min="2" max="2" width="7.85546875" customWidth="true"/>
     <col min="3" max="3" width="4.5703125" customWidth="true"/>
     <col min="4" max="4" width="4.85546875" customWidth="true"/>
     <col min="5" max="5" width="11.7109375" customWidth="true"/>
-    <col min="6" max="6" width="11.7109375" customWidth="true"/>
+    <col min="6" max="6" width="12.7109375" customWidth="true"/>
     <col min="7" max="7" width="11.7109375" customWidth="true"/>
     <col min="8" max="8" width="5" customWidth="true"/>
     <col min="9" max="9" width="12.85546875" customWidth="true"/>
@@ -265,7 +265,7 @@
     </row>
     <row r="2">
       <c r="A2" s="0" t="s">
-        <v>31</v>
+        <v>42</v>
       </c>
       <c r="B2" s="0">
         <v>90</v>
@@ -277,13 +277,13 @@
         <v>180</v>
       </c>
       <c r="E2" s="0">
-        <v>6.0773480662983426</v>
+        <v>3.3149171270718232</v>
       </c>
       <c r="F2" s="0">
-        <v>11.602209944751381</v>
+        <v>6.0773480662983426</v>
       </c>
       <c r="G2" s="0">
-        <v>83.425414364640886</v>
+        <v>91.712707182320443</v>
       </c>
       <c r="H2" s="0">
         <v>0</v>
@@ -294,7 +294,7 @@
     </row>
     <row r="3">
       <c r="A3" s="0" t="s">
-        <v>32</v>
+        <v>43</v>
       </c>
       <c r="B3" s="0">
         <v>90</v>
@@ -306,13 +306,13 @@
         <v>180</v>
       </c>
       <c r="E3" s="0">
-        <v>6.0773480662983426</v>
+        <v>3.3149171270718232</v>
       </c>
       <c r="F3" s="0">
-        <v>11.602209944751381</v>
+        <v>6.0773480662983426</v>
       </c>
       <c r="G3" s="0">
-        <v>83.425414364640886</v>
+        <v>91.712707182320443</v>
       </c>
       <c r="H3" s="0">
         <v>0</v>
@@ -323,7 +323,7 @@
     </row>
     <row r="4">
       <c r="A4" s="0" t="s">
-        <v>33</v>
+        <v>44</v>
       </c>
       <c r="B4" s="0">
         <v>90</v>
@@ -335,110 +335,236 @@
         <v>180</v>
       </c>
       <c r="E4" s="0">
-        <v>6.0773480662983426</v>
+        <v>3.3149171270718232</v>
       </c>
       <c r="F4" s="0">
+        <v>6.0773480662983426</v>
+      </c>
+      <c r="G4" s="0">
+        <v>91.712707182320443</v>
+      </c>
+      <c r="H4" s="0">
+        <v>0</v>
+      </c>
+      <c r="I4" s="0">
+        <v>101.10497237569061</v>
+      </c>
+    </row>
+    <row r="5">
+      <c r="A5" s="0" t="s">
+        <v>45</v>
+      </c>
+      <c r="B5" s="0">
+        <v>90</v>
+      </c>
+      <c r="C5" s="0">
+        <v>0</v>
+      </c>
+      <c r="D5" s="0">
+        <v>180</v>
+      </c>
+      <c r="E5" s="0">
+        <v>3.3149171270718232</v>
+      </c>
+      <c r="F5" s="0">
+        <v>0.55248618784530379</v>
+      </c>
+      <c r="G5" s="0">
+        <v>97.237569060773481</v>
+      </c>
+      <c r="H5" s="0">
+        <v>0</v>
+      </c>
+      <c r="I5" s="0">
+        <v>101.10497237569061</v>
+      </c>
+    </row>
+    <row r="6">
+      <c r="A6" s="0" t="s">
+        <v>46</v>
+      </c>
+      <c r="B6" s="0">
+        <v>90</v>
+      </c>
+      <c r="C6" s="0">
+        <v>0</v>
+      </c>
+      <c r="D6" s="0">
+        <v>180</v>
+      </c>
+      <c r="E6" s="0">
+        <v>3.3149171270718232</v>
+      </c>
+      <c r="F6" s="0">
+        <v>0.55248618784530379</v>
+      </c>
+      <c r="G6" s="0">
+        <v>97.237569060773481</v>
+      </c>
+      <c r="H6" s="0">
+        <v>0</v>
+      </c>
+      <c r="I6" s="0">
+        <v>101.10497237569061</v>
+      </c>
+    </row>
+    <row r="7">
+      <c r="A7" s="0" t="s">
+        <v>47</v>
+      </c>
+      <c r="B7" s="0">
+        <v>90</v>
+      </c>
+      <c r="C7" s="0">
+        <v>0</v>
+      </c>
+      <c r="D7" s="0">
+        <v>180</v>
+      </c>
+      <c r="E7" s="0">
+        <v>3.3149171270718232</v>
+      </c>
+      <c r="F7" s="0">
+        <v>0.55248618784530379</v>
+      </c>
+      <c r="G7" s="0">
+        <v>97.237569060773481</v>
+      </c>
+      <c r="H7" s="0">
+        <v>0</v>
+      </c>
+      <c r="I7" s="0">
+        <v>101.10497237569061</v>
+      </c>
+    </row>
+    <row r="8">
+      <c r="A8" s="0" t="s">
+        <v>4</v>
+      </c>
+      <c r="B8" s="0">
+        <v>90</v>
+      </c>
+      <c r="C8" s="0">
+        <v>0</v>
+      </c>
+      <c r="D8" s="0">
+        <v>180</v>
+      </c>
+      <c r="E8" s="0">
         <v>11.602209944751381</v>
       </c>
-      <c r="G4" s="0">
-        <v>83.425414364640886</v>
-      </c>
-      <c r="H4" s="0">
-        <v>0</v>
-      </c>
-      <c r="I4" s="0">
-        <v>101.10497237569061</v>
-      </c>
-    </row>
-    <row r="5">
-      <c r="A5" s="0"/>
-      <c r="B5" s="0"/>
-      <c r="C5" s="0"/>
-      <c r="D5" s="0"/>
-      <c r="E5" s="0"/>
-      <c r="F5" s="0"/>
-      <c r="G5" s="0"/>
-      <c r="H5" s="0"/>
-      <c r="I5" s="0"/>
-    </row>
-    <row r="6">
-      <c r="A6" s="0"/>
-      <c r="B6" s="0"/>
-      <c r="C6" s="0"/>
-      <c r="D6" s="0"/>
-      <c r="E6" s="0"/>
-      <c r="F6" s="0"/>
-      <c r="G6" s="0"/>
-      <c r="H6" s="0"/>
-      <c r="I6" s="0"/>
-    </row>
-    <row r="7">
-      <c r="A7" s="0"/>
-      <c r="B7" s="0"/>
-      <c r="C7" s="0"/>
-      <c r="D7" s="0"/>
-      <c r="E7" s="0"/>
-      <c r="F7" s="0"/>
-      <c r="G7" s="0"/>
-      <c r="H7" s="0"/>
-      <c r="I7" s="0"/>
-    </row>
-    <row r="8">
-      <c r="A8" s="0"/>
-      <c r="B8" s="0"/>
-      <c r="C8" s="0"/>
-      <c r="D8" s="0"/>
-      <c r="E8" s="0"/>
-      <c r="F8" s="0"/>
-      <c r="G8" s="0"/>
-      <c r="H8" s="0"/>
-      <c r="I8" s="0"/>
+      <c r="F8" s="0">
+        <v>22.651933701657459</v>
+      </c>
+      <c r="G8" s="0">
+        <v>66.850828729281758</v>
+      </c>
+      <c r="H8" s="0">
+        <v>0</v>
+      </c>
+      <c r="I8" s="0">
+        <v>101.10497237569061</v>
+      </c>
     </row>
     <row r="9">
-      <c r="A9" s="0"/>
-      <c r="B9" s="0"/>
-      <c r="C9" s="0"/>
-      <c r="D9" s="0"/>
-      <c r="E9" s="0"/>
-      <c r="F9" s="0"/>
-      <c r="G9" s="0"/>
-      <c r="H9" s="0"/>
-      <c r="I9" s="0"/>
+      <c r="A9" s="0" t="s">
+        <v>5</v>
+      </c>
+      <c r="B9" s="0">
+        <v>90</v>
+      </c>
+      <c r="C9" s="0">
+        <v>0</v>
+      </c>
+      <c r="D9" s="0">
+        <v>180</v>
+      </c>
+      <c r="E9" s="0">
+        <v>11.602209944751381</v>
+      </c>
+      <c r="F9" s="0">
+        <v>22.651933701657459</v>
+      </c>
+      <c r="G9" s="0">
+        <v>66.850828729281758</v>
+      </c>
+      <c r="H9" s="0">
+        <v>0</v>
+      </c>
+      <c r="I9" s="0">
+        <v>101.10497237569061</v>
+      </c>
     </row>
     <row r="10">
-      <c r="A10" s="0"/>
-      <c r="B10" s="0"/>
-      <c r="C10" s="0"/>
-      <c r="D10" s="0"/>
-      <c r="E10" s="0"/>
-      <c r="F10" s="0"/>
-      <c r="G10" s="0"/>
-      <c r="H10" s="0"/>
-      <c r="I10" s="0"/>
+      <c r="A10" s="0" t="s">
+        <v>6</v>
+      </c>
+      <c r="B10" s="0">
+        <v>90</v>
+      </c>
+      <c r="C10" s="0">
+        <v>0</v>
+      </c>
+      <c r="D10" s="0">
+        <v>180</v>
+      </c>
+      <c r="E10" s="0">
+        <v>11.602209944751381</v>
+      </c>
+      <c r="F10" s="0">
+        <v>22.651933701657459</v>
+      </c>
+      <c r="G10" s="0">
+        <v>66.850828729281758</v>
+      </c>
+      <c r="H10" s="0">
+        <v>0</v>
+      </c>
+      <c r="I10" s="0">
+        <v>101.10497237569061</v>
+      </c>
     </row>
     <row r="11">
-      <c r="A11" s="0"/>
-      <c r="B11" s="0"/>
-      <c r="C11" s="0"/>
-      <c r="D11" s="0"/>
-      <c r="E11" s="0"/>
-      <c r="F11" s="0"/>
-      <c r="G11" s="0"/>
-      <c r="H11" s="0"/>
-      <c r="I11" s="0"/>
+      <c r="A11" s="0" t="s">
+        <v>7</v>
+      </c>
+      <c r="B11" s="0">
+        <v>90</v>
+      </c>
+      <c r="C11" s="0">
+        <v>0</v>
+      </c>
+      <c r="D11" s="0">
+        <v>180</v>
+      </c>
+      <c r="E11" s="0">
+        <v>0</v>
+      </c>
+      <c r="F11" s="0">
+        <v>0</v>
+      </c>
+      <c r="G11" s="0">
+        <v>0</v>
+      </c>
+      <c r="H11" s="0">
+        <v>0</v>
+      </c>
+      <c r="I11" s="0">
+        <v>0</v>
+      </c>
     </row>
     <row r="12">
       <c r="A12" s="0" t="s">
         <v>8</v>
       </c>
       <c r="B12" s="0">
-        <v>67.035729272602353</v>
+        <v>90</v>
       </c>
       <c r="C12" s="0">
-        <v>-65.772343902386694</v>
+        <v>0</v>
       </c>
       <c r="D12" s="0">
-        <v>174.73185673422799</v>
+        <v>180</v>
       </c>
       <c r="E12" s="0">
         <v>0</v>
@@ -461,13 +587,13 @@
         <v>9</v>
       </c>
       <c r="B13" s="0">
-        <v>44.222785814108704</v>
+        <v>90</v>
       </c>
       <c r="C13" s="0">
-        <v>-52.468041020853804</v>
+        <v>0</v>
       </c>
       <c r="D13" s="0">
-        <v>159.98850067244601</v>
+        <v>180</v>
       </c>
       <c r="E13" s="0">
         <v>0</v>
@@ -490,28 +616,28 @@
         <v>10</v>
       </c>
       <c r="B14" s="0">
-        <v>5.5241928379928957</v>
+        <v>90</v>
       </c>
       <c r="C14" s="0">
-        <v>-89.425096386377106</v>
+        <v>0</v>
       </c>
       <c r="D14" s="0">
-        <v>87.583824191846503</v>
+        <v>180</v>
       </c>
       <c r="E14" s="0">
-        <v>4.8206278026905833</v>
+        <v>3.3149171270718232</v>
       </c>
       <c r="F14" s="0">
-        <v>8.7331838565022419</v>
+        <v>6.0773480662983426</v>
       </c>
       <c r="G14" s="0">
-        <v>41.72645739910314</v>
+        <v>91.712707182320443</v>
       </c>
       <c r="H14" s="0">
         <v>0</v>
       </c>
       <c r="I14" s="0">
-        <v>55.280269058295964</v>
+        <v>101.10497237569061</v>
       </c>
     </row>
     <row r="15">
@@ -519,28 +645,28 @@
         <v>11</v>
       </c>
       <c r="B15" s="0">
-        <v>42.217495777057451</v>
+        <v>90</v>
       </c>
       <c r="C15" s="0">
-        <v>-179.599138863013</v>
+        <v>0</v>
       </c>
       <c r="D15" s="0">
-        <v>179.490232518791</v>
+        <v>180</v>
       </c>
       <c r="E15" s="0">
-        <v>2.9596412556053813</v>
+        <v>3.3149171270718232</v>
       </c>
       <c r="F15" s="0">
-        <v>5.2802690582959642</v>
+        <v>6.0773480662983426</v>
       </c>
       <c r="G15" s="0">
-        <v>66.087443946188344</v>
+        <v>91.712707182320443</v>
       </c>
       <c r="H15" s="0">
         <v>0</v>
       </c>
       <c r="I15" s="0">
-        <v>74.327354260089692</v>
+        <v>101.10497237569061</v>
       </c>
     </row>
     <row r="16">
@@ -548,28 +674,28 @@
         <v>12</v>
       </c>
       <c r="B16" s="0">
-        <v>-21.810325391650149</v>
+        <v>90</v>
       </c>
       <c r="C16" s="0">
-        <v>-179.99997391993301</v>
+        <v>0</v>
       </c>
       <c r="D16" s="0">
-        <v>179.77469146537999</v>
+        <v>180</v>
       </c>
       <c r="E16" s="0">
-        <v>5.1793721973094167</v>
+        <v>3.3149171270718232</v>
       </c>
       <c r="F16" s="0">
-        <v>6.7152466367713011</v>
+        <v>6.0773480662983426</v>
       </c>
       <c r="G16" s="0">
-        <v>17.892376681614351</v>
+        <v>91.712707182320443</v>
       </c>
       <c r="H16" s="0">
         <v>0</v>
       </c>
       <c r="I16" s="0">
-        <v>29.786995515695068</v>
+        <v>101.10497237569061</v>
       </c>
     </row>
     <row r="17">
@@ -577,28 +703,28 @@
         <v>13</v>
       </c>
       <c r="B17" s="0">
-        <v>7.740036771974105</v>
+        <v>90</v>
       </c>
       <c r="C17" s="0">
-        <v>-21.820556950950401</v>
+        <v>0</v>
       </c>
       <c r="D17" s="0">
-        <v>47.036644219330299</v>
+        <v>180</v>
       </c>
       <c r="E17" s="0">
-        <v>0</v>
+        <v>11.602209944751381</v>
       </c>
       <c r="F17" s="0">
-        <v>8.3071748878923763</v>
+        <v>22.651933701657459</v>
       </c>
       <c r="G17" s="0">
-        <v>0</v>
+        <v>66.850828729281758</v>
       </c>
       <c r="H17" s="0">
-        <v>82.612107623318394</v>
+        <v>0</v>
       </c>
       <c r="I17" s="0">
-        <v>8.3071748878923763</v>
+        <v>101.10497237569061</v>
       </c>
     </row>
     <row r="18">
@@ -606,28 +732,28 @@
         <v>14</v>
       </c>
       <c r="B18" s="0">
-        <v>13.7713796105868</v>
+        <v>90</v>
       </c>
       <c r="C18" s="0">
-        <v>-43.728449213337299</v>
+        <v>0</v>
       </c>
       <c r="D18" s="0">
-        <v>56.908493492938</v>
+        <v>180</v>
       </c>
       <c r="E18" s="0">
-        <v>0</v>
+        <v>11.602209944751381</v>
       </c>
       <c r="F18" s="0">
-        <v>37.959641255605383</v>
+        <v>22.651933701657459</v>
       </c>
       <c r="G18" s="0">
-        <v>0</v>
+        <v>66.850828729281758</v>
       </c>
       <c r="H18" s="0">
-        <v>41.00896860986547</v>
+        <v>0</v>
       </c>
       <c r="I18" s="0">
-        <v>37.959641255605383</v>
+        <v>101.10497237569061</v>
       </c>
     </row>
     <row r="19">
@@ -635,28 +761,28 @@
         <v>15</v>
       </c>
       <c r="B19" s="0">
-        <v>21.9341946313397</v>
+        <v>90</v>
       </c>
       <c r="C19" s="0">
-        <v>-44.891381586050301</v>
+        <v>0</v>
       </c>
       <c r="D19" s="0">
-        <v>83.838028371070294</v>
+        <v>180</v>
       </c>
       <c r="E19" s="0">
-        <v>39.091928251121075</v>
+        <v>11.602209944751381</v>
       </c>
       <c r="F19" s="0">
-        <v>51.872197309417047</v>
+        <v>22.651933701657459</v>
       </c>
       <c r="G19" s="0">
-        <v>4.2264573991031389</v>
+        <v>66.850828729281758</v>
       </c>
       <c r="H19" s="0">
         <v>0</v>
       </c>
       <c r="I19" s="0">
-        <v>95.190582959641262</v>
+        <v>101.10497237569061</v>
       </c>
     </row>
     <row r="20">
@@ -664,13 +790,13 @@
         <v>16</v>
       </c>
       <c r="B20" s="0">
-        <v>-9.5844571068494062</v>
+        <v>90</v>
       </c>
       <c r="C20" s="0">
-        <v>-75.485737677646497</v>
+        <v>0</v>
       </c>
       <c r="D20" s="0">
-        <v>35.539988122927497</v>
+        <v>180</v>
       </c>
       <c r="E20" s="0">
         <v>0</v>
@@ -693,13 +819,13 @@
         <v>17</v>
       </c>
       <c r="B21" s="0">
-        <v>66.030571124831695</v>
+        <v>90</v>
       </c>
       <c r="C21" s="0">
-        <v>-31.923995841788599</v>
+        <v>0</v>
       </c>
       <c r="D21" s="0">
-        <v>137.96940114528701</v>
+        <v>180</v>
       </c>
       <c r="E21" s="0">
         <v>0</v>
@@ -722,13 +848,13 @@
         <v>18</v>
       </c>
       <c r="B22" s="0">
-        <v>47.877689839817904</v>
+        <v>90</v>
       </c>
       <c r="C22" s="0">
-        <v>-13.3801218979171</v>
+        <v>0</v>
       </c>
       <c r="D22" s="0">
-        <v>152.42691614070401</v>
+        <v>180</v>
       </c>
       <c r="E22" s="0">
         <v>0</v>
@@ -751,28 +877,28 @@
         <v>19</v>
       </c>
       <c r="B23" s="0">
-        <v>3.1766172690525947</v>
+        <v>90</v>
       </c>
       <c r="C23" s="0">
-        <v>-83.945123560199306</v>
+        <v>0</v>
       </c>
       <c r="D23" s="0">
-        <v>87.341748097180002</v>
+        <v>180</v>
       </c>
       <c r="E23" s="0">
-        <v>6.3452914798206281</v>
+        <v>3.3149171270718232</v>
       </c>
       <c r="F23" s="0">
-        <v>9.1928251121076237</v>
+        <v>6.0773480662983426</v>
       </c>
       <c r="G23" s="0">
-        <v>39.248878923766817</v>
+        <v>91.712707182320443</v>
       </c>
       <c r="H23" s="0">
         <v>0</v>
       </c>
       <c r="I23" s="0">
-        <v>54.786995515695068</v>
+        <v>101.10497237569061</v>
       </c>
     </row>
     <row r="24">
@@ -780,28 +906,28 @@
         <v>20</v>
       </c>
       <c r="B24" s="0">
-        <v>54.950154444605346</v>
+        <v>90</v>
       </c>
       <c r="C24" s="0">
-        <v>-179.99462121883499</v>
+        <v>0</v>
       </c>
       <c r="D24" s="0">
-        <v>179.965373349917</v>
+        <v>180</v>
       </c>
       <c r="E24" s="0">
-        <v>2.8026905829596416</v>
+        <v>3.3149171270718232</v>
       </c>
       <c r="F24" s="0">
-        <v>4.6524663677130045</v>
+        <v>6.0773480662983426</v>
       </c>
       <c r="G24" s="0">
-        <v>71.692825112107627</v>
+        <v>91.712707182320443</v>
       </c>
       <c r="H24" s="0">
         <v>0</v>
       </c>
       <c r="I24" s="0">
-        <v>79.147982062780272</v>
+        <v>101.10497237569061</v>
       </c>
     </row>
     <row r="25">
@@ -809,28 +935,28 @@
         <v>21</v>
       </c>
       <c r="B25" s="0">
-        <v>-23.730004712883851</v>
+        <v>90</v>
       </c>
       <c r="C25" s="0">
-        <v>-179.936453743854</v>
+        <v>0</v>
       </c>
       <c r="D25" s="0">
-        <v>179.81342543044599</v>
+        <v>180</v>
       </c>
       <c r="E25" s="0">
-        <v>4.506726457399103</v>
+        <v>3.3149171270718232</v>
       </c>
       <c r="F25" s="0">
-        <v>7.7690582959641246</v>
+        <v>6.0773480662983426</v>
       </c>
       <c r="G25" s="0">
-        <v>19.663677130044842</v>
+        <v>91.712707182320443</v>
       </c>
       <c r="H25" s="0">
         <v>0</v>
       </c>
       <c r="I25" s="0">
-        <v>31.939461883408072</v>
+        <v>101.10497237569061</v>
       </c>
     </row>
     <row r="26">
@@ -838,28 +964,28 @@
         <v>25</v>
       </c>
       <c r="B26" s="0">
-        <v>0.49284560359171647</v>
+        <v>90</v>
       </c>
       <c r="C26" s="0">
-        <v>-4.6519779611746497</v>
+        <v>0</v>
       </c>
       <c r="D26" s="0">
-        <v>15.575183350311899</v>
+        <v>180</v>
       </c>
       <c r="E26" s="0">
-        <v>0</v>
+        <v>6.0773480662983426</v>
       </c>
       <c r="F26" s="0">
-        <v>0.51569506726457404</v>
+        <v>11.602209944751381</v>
       </c>
       <c r="G26" s="0">
-        <v>0</v>
+        <v>83.425414364640886</v>
       </c>
       <c r="H26" s="0">
-        <v>57.051569506726466</v>
+        <v>0</v>
       </c>
       <c r="I26" s="0">
-        <v>0.51569506726457404</v>
+        <v>101.10497237569061</v>
       </c>
     </row>
     <row r="27">
@@ -867,28 +993,28 @@
         <v>26</v>
       </c>
       <c r="B27" s="0">
-        <v>-0.40739721701834453</v>
+        <v>90</v>
       </c>
       <c r="C27" s="0">
-        <v>-15.108827970097</v>
+        <v>0</v>
       </c>
       <c r="D27" s="0">
-        <v>17.911360789958199</v>
+        <v>180</v>
       </c>
       <c r="E27" s="0">
-        <v>0</v>
+        <v>6.0773480662983426</v>
       </c>
       <c r="F27" s="0">
-        <v>3.2511210762331837</v>
+        <v>11.602209944751381</v>
       </c>
       <c r="G27" s="0">
-        <v>0</v>
+        <v>83.425414364640886</v>
       </c>
       <c r="H27" s="0">
-        <v>43.531390134529147</v>
+        <v>0</v>
       </c>
       <c r="I27" s="0">
-        <v>3.2511210762331837</v>
+        <v>101.10497237569061</v>
       </c>
     </row>
     <row r="28">
@@ -896,28 +1022,28 @@
         <v>27</v>
       </c>
       <c r="B28" s="0">
-        <v>15.371605156493949</v>
+        <v>90</v>
       </c>
       <c r="C28" s="0">
-        <v>-3.7418584013920002</v>
+        <v>0</v>
       </c>
       <c r="D28" s="0">
-        <v>155.397247334941</v>
+        <v>180</v>
       </c>
       <c r="E28" s="0">
-        <v>36.121076233183857</v>
+        <v>6.0773480662983426</v>
       </c>
       <c r="F28" s="0">
-        <v>48.56502242152466</v>
+        <v>11.602209944751381</v>
       </c>
       <c r="G28" s="0">
-        <v>14.260089686098654</v>
+        <v>83.425414364640886</v>
       </c>
       <c r="H28" s="0">
         <v>0</v>
       </c>
       <c r="I28" s="0">
-        <v>98.946188340807169</v>
+        <v>101.10497237569061</v>
       </c>
     </row>
     <row r="29">
@@ -925,28 +1051,28 @@
         <v>31</v>
       </c>
       <c r="B29" s="0">
-        <v>-0.08530494418099005</v>
+        <v>90</v>
       </c>
       <c r="C29" s="0">
-        <v>-10.165825057581699</v>
+        <v>0</v>
       </c>
       <c r="D29" s="0">
-        <v>11.8575857434467</v>
+        <v>180</v>
       </c>
       <c r="E29" s="0">
-        <v>0</v>
+        <v>6.0773480662983426</v>
       </c>
       <c r="F29" s="0">
-        <v>0.2802690582959641</v>
+        <v>11.602209944751381</v>
       </c>
       <c r="G29" s="0">
-        <v>0</v>
+        <v>83.425414364640886</v>
       </c>
       <c r="H29" s="0">
-        <v>48.206278026905828</v>
+        <v>0</v>
       </c>
       <c r="I29" s="0">
-        <v>0.2802690582959641</v>
+        <v>101.10497237569061</v>
       </c>
     </row>
     <row r="30">
@@ -954,28 +1080,28 @@
         <v>32</v>
       </c>
       <c r="B30" s="0">
-        <v>-0.83586032287941747</v>
+        <v>90</v>
       </c>
       <c r="C30" s="0">
-        <v>-17.5751832524092</v>
+        <v>0</v>
       </c>
       <c r="D30" s="0">
-        <v>18.901197932947198</v>
+        <v>180</v>
       </c>
       <c r="E30" s="0">
-        <v>0</v>
+        <v>6.0773480662983426</v>
       </c>
       <c r="F30" s="0">
-        <v>2.5</v>
+        <v>11.602209944751381</v>
       </c>
       <c r="G30" s="0">
-        <v>0</v>
+        <v>83.425414364640886</v>
       </c>
       <c r="H30" s="0">
-        <v>37.040358744394617</v>
+        <v>0</v>
       </c>
       <c r="I30" s="0">
-        <v>2.5</v>
+        <v>101.10497237569061</v>
       </c>
     </row>
     <row r="31">
@@ -983,28 +1109,28 @@
         <v>33</v>
       </c>
       <c r="B31" s="0">
-        <v>16.580742738412852</v>
+        <v>90</v>
       </c>
       <c r="C31" s="0">
-        <v>1.03325845525986</v>
+        <v>0</v>
       </c>
       <c r="D31" s="0">
-        <v>156.51753593351799</v>
+        <v>180</v>
       </c>
       <c r="E31" s="0">
-        <v>32.253363228699548</v>
+        <v>6.0773480662983426</v>
       </c>
       <c r="F31" s="0">
-        <v>47.600896860986545</v>
+        <v>11.602209944751381</v>
       </c>
       <c r="G31" s="0">
-        <v>20.1457399103139</v>
+        <v>83.425414364640886</v>
       </c>
       <c r="H31" s="0">
         <v>0</v>
       </c>
       <c r="I31" s="0">
-        <v>100</v>
+        <v>101.10497237569061</v>
       </c>
     </row>
     <row r="32">

</xml_diff>